<commit_message>
grado 08, actualización viernes
hasta antes de lectura de Carlos, que la finaliza esta tarde (guion 05).
Revisión inicial mía de guion 06
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Chequeo de recursos CS_08_05.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Chequeo de recursos CS_08_05.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCMarquez\Desktop\RECURSOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flor\Documents\Trabajo Ed Planeta\CienciasSociales\fuentes\contenidos\grado08\guion05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="6675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Código del guion</t>
   </si>
@@ -67,6 +67,72 @@
   </si>
   <si>
     <t>Autor</t>
+  </si>
+  <si>
+    <t>CS_08_05_CO</t>
+  </si>
+  <si>
+    <t>REC10</t>
+  </si>
+  <si>
+    <t>REC20</t>
+  </si>
+  <si>
+    <t>REC30</t>
+  </si>
+  <si>
+    <t>REC40</t>
+  </si>
+  <si>
+    <t>REC50</t>
+  </si>
+  <si>
+    <t>REC60</t>
+  </si>
+  <si>
+    <t>REC70</t>
+  </si>
+  <si>
+    <t>REC80</t>
+  </si>
+  <si>
+    <t>REC90</t>
+  </si>
+  <si>
+    <t>REC100</t>
+  </si>
+  <si>
+    <t>REC110</t>
+  </si>
+  <si>
+    <t>REC120</t>
+  </si>
+  <si>
+    <t>REC130</t>
+  </si>
+  <si>
+    <t>REC140</t>
+  </si>
+  <si>
+    <t>REC150</t>
+  </si>
+  <si>
+    <t>REC160</t>
+  </si>
+  <si>
+    <t>REC170</t>
+  </si>
+  <si>
+    <t>REC180</t>
+  </si>
+  <si>
+    <t>REC190</t>
+  </si>
+  <si>
+    <t>REC200</t>
+  </si>
+  <si>
+    <t>REC210</t>
   </si>
 </sst>
 </file>
@@ -393,20 +459,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" customWidth="1"/>
   </cols>
@@ -444,6 +512,114 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>